<commit_message>
new constraint: the third wheel
</commit_message>
<xml_diff>
--- a/excel/germany/season ?/night_7.xlsx
+++ b/excel/germany/season ?/night_7.xlsx
@@ -55,7 +55,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill/>
     </fill>
@@ -96,16 +96,6 @@
         <fgColor rgb="0000a933"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00aad761"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00ff9e50"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -133,7 +123,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -198,22 +188,10 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -580,10 +558,10 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="17.66" customWidth="1" style="11" min="1" max="1"/>
   </cols>
@@ -853,6 +831,28 @@
       <c r="J13" s="13" t="n"/>
       <c r="K13" s="13" t="n"/>
       <c r="L13" s="13" t="n"/>
+    </row>
+    <row r="14" ht="12.8" customHeight="1" s="12">
+      <c r="A14" s="13" t="n"/>
+      <c r="B14" s="13" t="n"/>
+      <c r="C14" s="13" t="n"/>
+    </row>
+    <row r="15" ht="12.8" customHeight="1" s="12">
+      <c r="A15" s="13" t="inlineStr">
+        <is>
+          <t>Third wheel:</t>
+        </is>
+      </c>
+      <c r="B15" s="11">
+        <f>A4</f>
+        <v/>
+      </c>
+      <c r="C15" s="13" t="n"/>
+    </row>
+    <row r="16" ht="12.8" customHeight="1" s="12">
+      <c r="A16" s="13" t="n"/>
+      <c r="B16" s="13" t="n"/>
+      <c r="C16" s="13" t="n"/>
     </row>
     <row r="17" ht="12.8" customHeight="1" s="12">
       <c r="A17" s="13" t="n"/>
@@ -1989,10 +1989,10 @@
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.7578125" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.78515625" defaultRowHeight="12.75" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="17.66" customWidth="1" style="11" min="1" max="1"/>
   </cols>
@@ -2120,9 +2120,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="C3" s="22" t="inlineStr">
-        <is>
-          <t>66.67%</t>
+      <c r="C3" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D3" s="20" t="inlineStr">
@@ -2135,9 +2135,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="F3" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="F3" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="G3" s="20" t="inlineStr">
@@ -2173,14 +2173,14 @@
           <t>Dana</t>
         </is>
       </c>
-      <c r="B4" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="C4" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="B4" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="C4" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="D4" s="20" t="inlineStr">
@@ -2218,9 +2218,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="K4" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="K4" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="L4" s="13" t="n"/>
@@ -2289,9 +2289,9 @@
           <t>Gabriela</t>
         </is>
       </c>
-      <c r="B6" s="22" t="inlineStr">
-        <is>
-          <t>66.67%</t>
+      <c r="B6" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="C6" s="20" t="inlineStr">
@@ -2309,9 +2309,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="F6" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="F6" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="G6" s="20" t="inlineStr">
@@ -2362,14 +2362,14 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="E7" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="F7" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="E7" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="F7" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="G7" s="20" t="inlineStr">
@@ -2377,9 +2377,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="H7" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="H7" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="I7" s="20" t="inlineStr">
@@ -2488,14 +2488,14 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="G9" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
-        </is>
-      </c>
-      <c r="H9" s="22" t="inlineStr">
-        <is>
-          <t>66.67%</t>
+      <c r="G9" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
+        </is>
+      </c>
+      <c r="H9" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="I9" s="20" t="inlineStr">
@@ -2594,9 +2594,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="E11" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="E11" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="F11" s="20" t="inlineStr">
@@ -2604,9 +2604,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="G11" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="G11" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="H11" s="20" t="inlineStr">
@@ -2614,9 +2614,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="I11" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="I11" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="J11" s="20" t="inlineStr">
@@ -2652,9 +2652,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="E12" s="22" t="inlineStr">
-        <is>
-          <t>66.67%</t>
+      <c r="E12" s="20" t="inlineStr">
+        <is>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="F12" s="20" t="inlineStr">
@@ -2662,9 +2662,9 @@
           <t>0.0%</t>
         </is>
       </c>
-      <c r="G12" s="23" t="inlineStr">
-        <is>
-          <t>33.33%</t>
+      <c r="G12" s="21" t="inlineStr">
+        <is>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="H12" s="20" t="inlineStr">
@@ -2702,6 +2702,28 @@
       <c r="J13" s="13" t="n"/>
       <c r="K13" s="13" t="n"/>
       <c r="L13" s="13" t="n"/>
+    </row>
+    <row r="14" ht="12.8" customHeight="1" s="12">
+      <c r="A14" s="13" t="n"/>
+      <c r="B14" s="13" t="n"/>
+      <c r="C14" s="13" t="n"/>
+    </row>
+    <row r="15" ht="12.8" customHeight="1" s="12">
+      <c r="A15" s="13" t="inlineStr">
+        <is>
+          <t>Third wheel:</t>
+        </is>
+      </c>
+      <c r="B15" s="11">
+        <f>Input!B15</f>
+        <v/>
+      </c>
+      <c r="C15" s="13" t="n"/>
+    </row>
+    <row r="16" ht="12.8" customHeight="1" s="12">
+      <c r="A16" s="13" t="n"/>
+      <c r="B16" s="13" t="n"/>
+      <c r="C16" s="13" t="n"/>
     </row>
     <row r="17" ht="12.8" customHeight="1" s="12">
       <c r="A17" s="13" t="n"/>
@@ -2805,102 +2827,102 @@
       <c r="A19" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="B19" s="24" t="inlineStr">
+      <c r="B19" s="22" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C19" s="24" t="inlineStr">
+      <c r="C19" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="D19" s="25" t="inlineStr">
+      <c r="D19" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E19" s="25" t="inlineStr">
+      <c r="E19" s="23" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="F19" s="24" t="inlineStr">
+      <c r="F19" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G19" s="24" t="inlineStr">
+      <c r="G19" s="22" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="H19" s="24" t="inlineStr">
+      <c r="H19" s="22" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I19" s="24" t="inlineStr">
+      <c r="I19" s="22" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
       </c>
-      <c r="J19" s="24" t="inlineStr">
+      <c r="J19" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K19" s="24" t="inlineStr">
+      <c r="K19" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="L19" s="25" t="inlineStr">
+      <c r="L19" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M19" s="25" t="inlineStr">
+      <c r="M19" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N19" s="24" t="inlineStr">
+      <c r="N19" s="22" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O19" s="24" t="inlineStr">
+      <c r="O19" s="22" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="P19" s="24" t="inlineStr">
+      <c r="P19" s="22" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q19" s="24" t="inlineStr">
+      <c r="Q19" s="22" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="R19" s="24" t="inlineStr">
+      <c r="R19" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S19" s="24" t="inlineStr">
+      <c r="S19" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="T19" s="24" t="inlineStr">
+      <c r="T19" s="22" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U19" s="24" t="inlineStr">
+      <c r="U19" s="22" t="inlineStr">
         <is>
           <t>Laura B</t>
         </is>
@@ -2914,102 +2936,102 @@
       <c r="A20" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="B20" s="24" t="inlineStr">
+      <c r="B20" s="22" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C20" s="24" t="inlineStr">
+      <c r="C20" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="D20" s="25" t="inlineStr">
+      <c r="D20" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E20" s="25" t="inlineStr">
+      <c r="E20" s="23" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="F20" s="26" t="inlineStr">
+      <c r="F20" s="23" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G20" s="26" t="inlineStr">
+      <c r="G20" s="23" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="H20" s="24" t="inlineStr">
+      <c r="H20" s="22" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I20" s="24" t="inlineStr">
+      <c r="I20" s="22" t="inlineStr">
         <is>
           <t>Laura B</t>
         </is>
       </c>
-      <c r="J20" s="24" t="inlineStr">
+      <c r="J20" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K20" s="24" t="inlineStr">
+      <c r="K20" s="22" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="L20" s="25" t="inlineStr">
+      <c r="L20" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M20" s="25" t="inlineStr">
+      <c r="M20" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N20" s="26" t="inlineStr">
+      <c r="N20" s="22" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O20" s="26" t="inlineStr">
+      <c r="O20" s="22" t="inlineStr">
         <is>
           <t>Dana</t>
         </is>
       </c>
-      <c r="P20" s="24" t="inlineStr">
+      <c r="P20" s="22" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q20" s="24" t="inlineStr">
+      <c r="Q20" s="22" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="R20" s="26" t="inlineStr">
+      <c r="R20" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S20" s="26" t="inlineStr">
+      <c r="S20" s="22" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="T20" s="24" t="inlineStr">
+      <c r="T20" s="22" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U20" s="24" t="inlineStr">
+      <c r="U20" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
@@ -3023,102 +3045,102 @@
       <c r="A21" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="B21" s="25" t="inlineStr">
+      <c r="B21" s="23" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C21" s="25" t="inlineStr">
+      <c r="C21" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">Laura B </t>
         </is>
       </c>
-      <c r="D21" s="26" t="inlineStr">
+      <c r="D21" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E21" s="26" t="inlineStr">
+      <c r="E21" s="23" t="inlineStr">
         <is>
           <t>Dana</t>
         </is>
       </c>
-      <c r="F21" s="26" t="inlineStr">
+      <c r="F21" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G21" s="26" t="inlineStr">
+      <c r="G21" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="H21" s="24" t="inlineStr">
+      <c r="H21" s="22" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I21" s="24" t="inlineStr">
+      <c r="I21" s="22" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="J21" s="26" t="inlineStr">
+      <c r="J21" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K21" s="26" t="inlineStr">
+      <c r="K21" s="22" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
       </c>
-      <c r="L21" s="25" t="inlineStr">
+      <c r="L21" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M21" s="25" t="inlineStr">
+      <c r="M21" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N21" s="24" t="inlineStr">
+      <c r="N21" s="22" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O21" s="24" t="inlineStr">
+      <c r="O21" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="P21" s="24" t="inlineStr">
+      <c r="P21" s="22" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q21" s="24" t="inlineStr">
+      <c r="Q21" s="22" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="R21" s="24" t="inlineStr">
+      <c r="R21" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S21" s="24" t="inlineStr">
+      <c r="S21" s="22" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="T21" s="24" t="inlineStr">
+      <c r="T21" s="22" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U21" s="24" t="inlineStr">
+      <c r="U21" s="22" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
@@ -3132,102 +3154,102 @@
       <c r="A22" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="B22" s="24" t="inlineStr">
+      <c r="B22" s="22" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C22" s="24" t="inlineStr">
+      <c r="C22" s="22" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="D22" s="24" t="inlineStr">
+      <c r="D22" s="22" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E22" s="24" t="inlineStr">
+      <c r="E22" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Laura B </t>
         </is>
       </c>
-      <c r="F22" s="24" t="inlineStr">
+      <c r="F22" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G22" s="24" t="inlineStr">
+      <c r="G22" s="22" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="H22" s="24" t="inlineStr">
+      <c r="H22" s="22" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I22" s="24" t="inlineStr">
+      <c r="I22" s="22" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="J22" s="24" t="inlineStr">
+      <c r="J22" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K22" s="24" t="inlineStr">
+      <c r="K22" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="L22" s="25" t="inlineStr">
+      <c r="L22" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M22" s="25" t="inlineStr">
+      <c r="M22" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N22" s="24" t="inlineStr">
+      <c r="N22" s="22" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O22" s="24" t="inlineStr">
+      <c r="O22" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="P22" s="24" t="inlineStr">
+      <c r="P22" s="22" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q22" s="24" t="inlineStr">
+      <c r="Q22" s="22" t="inlineStr">
         <is>
           <t xml:space="preserve">Linda </t>
         </is>
       </c>
-      <c r="R22" s="24" t="inlineStr">
+      <c r="R22" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S22" s="24" t="inlineStr">
+      <c r="S22" s="22" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
       </c>
-      <c r="T22" s="24" t="inlineStr">
+      <c r="T22" s="22" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U22" s="24" t="inlineStr">
+      <c r="U22" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
@@ -3241,102 +3263,102 @@
       <c r="A23" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="B23" s="25" t="inlineStr">
+      <c r="B23" s="23" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C23" s="25" t="inlineStr">
+      <c r="C23" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">Laura B </t>
         </is>
       </c>
-      <c r="D23" s="25" t="inlineStr">
+      <c r="D23" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E23" s="25" t="inlineStr">
+      <c r="E23" s="23" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="F23" s="27" t="inlineStr">
+      <c r="F23" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G23" s="27" t="inlineStr">
+      <c r="G23" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="H23" s="24" t="inlineStr">
+      <c r="H23" s="22" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I23" s="24" t="inlineStr">
+      <c r="I23" s="22" t="inlineStr">
         <is>
           <t>Dana</t>
         </is>
       </c>
-      <c r="J23" s="24" t="inlineStr">
+      <c r="J23" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K23" s="24" t="inlineStr">
+      <c r="K23" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="L23" s="25" t="inlineStr">
+      <c r="L23" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M23" s="25" t="inlineStr">
+      <c r="M23" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N23" s="27" t="inlineStr">
+      <c r="N23" s="23" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O23" s="27" t="inlineStr">
+      <c r="O23" s="23" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="P23" s="24" t="inlineStr">
+      <c r="P23" s="22" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q23" s="24" t="inlineStr">
+      <c r="Q23" s="22" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="R23" s="24" t="inlineStr">
+      <c r="R23" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S23" s="24" t="inlineStr">
+      <c r="S23" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="T23" s="27" t="inlineStr">
+      <c r="T23" s="23" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U23" s="27" t="inlineStr">
+      <c r="U23" s="23" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
@@ -3350,102 +3372,102 @@
       <c r="A24" s="13" t="n">
         <v>6</v>
       </c>
-      <c r="B24" s="26" t="inlineStr">
+      <c r="B24" s="22" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C24" s="26" t="inlineStr">
+      <c r="C24" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="D24" s="25" t="inlineStr">
+      <c r="D24" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E24" s="25" t="inlineStr">
+      <c r="E24" s="23" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="F24" s="27" t="inlineStr">
+      <c r="F24" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G24" s="27" t="inlineStr">
+      <c r="G24" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="H24" s="25" t="inlineStr">
+      <c r="H24" s="23" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I24" s="25" t="inlineStr">
+      <c r="I24" s="23" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="J24" s="24" t="inlineStr">
+      <c r="J24" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K24" s="24" t="inlineStr">
+      <c r="K24" s="22" t="inlineStr">
         <is>
           <t>Dana</t>
         </is>
       </c>
-      <c r="L24" s="25" t="inlineStr">
+      <c r="L24" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M24" s="25" t="inlineStr">
+      <c r="M24" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N24" s="27" t="inlineStr">
+      <c r="N24" s="23" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O24" s="27" t="inlineStr">
+      <c r="O24" s="23" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="P24" s="27" t="inlineStr">
+      <c r="P24" s="23" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q24" s="27" t="inlineStr">
+      <c r="Q24" s="23" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="R24" s="24" t="inlineStr">
+      <c r="R24" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S24" s="24" t="inlineStr">
+      <c r="S24" s="22" t="inlineStr">
         <is>
           <t>Jennifer</t>
         </is>
       </c>
-      <c r="T24" s="27" t="inlineStr">
+      <c r="T24" s="23" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U24" s="27" t="inlineStr">
+      <c r="U24" s="23" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
@@ -3459,102 +3481,102 @@
       <c r="A25" s="13" t="n">
         <v>7</v>
       </c>
-      <c r="B25" s="26" t="inlineStr">
+      <c r="B25" s="22" t="inlineStr">
         <is>
           <t>Nikola</t>
         </is>
       </c>
-      <c r="C25" s="26" t="inlineStr">
+      <c r="C25" s="22" t="inlineStr">
         <is>
           <t>Nadja</t>
         </is>
       </c>
-      <c r="D25" s="25" t="inlineStr">
+      <c r="D25" s="23" t="inlineStr">
         <is>
           <t>Tim</t>
         </is>
       </c>
-      <c r="E25" s="25" t="inlineStr">
+      <c r="E25" s="23" t="inlineStr">
         <is>
           <t>Linda</t>
         </is>
       </c>
-      <c r="F25" s="27" t="inlineStr">
+      <c r="F25" s="22" t="inlineStr">
         <is>
           <t>Kaan</t>
         </is>
       </c>
-      <c r="G25" s="27" t="inlineStr">
+      <c r="G25" s="22" t="inlineStr">
         <is>
           <t>Tara</t>
         </is>
       </c>
-      <c r="H25" s="25" t="inlineStr">
+      <c r="H25" s="23" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I25" s="25" t="inlineStr">
+      <c r="I25" s="23" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
       </c>
-      <c r="J25" s="24" t="inlineStr">
+      <c r="J25" s="22" t="inlineStr">
         <is>
           <t>Lars</t>
         </is>
       </c>
-      <c r="K25" s="24" t="inlineStr">
+      <c r="K25" s="22" t="inlineStr">
         <is>
           <t>Laura B</t>
         </is>
       </c>
-      <c r="L25" s="25" t="inlineStr">
+      <c r="L25" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M25" s="25" t="inlineStr">
+      <c r="M25" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
       </c>
-      <c r="N25" s="27" t="inlineStr">
+      <c r="N25" s="23" t="inlineStr">
         <is>
           <t>Antonino</t>
         </is>
       </c>
-      <c r="O25" s="27" t="inlineStr">
+      <c r="O25" s="23" t="inlineStr">
         <is>
           <t>Asena</t>
         </is>
       </c>
-      <c r="P25" s="27" t="inlineStr">
+      <c r="P25" s="23" t="inlineStr">
         <is>
           <t>Marc-Robin</t>
         </is>
       </c>
-      <c r="Q25" s="27" t="inlineStr">
+      <c r="Q25" s="23" t="inlineStr">
         <is>
           <t>Laura M</t>
         </is>
       </c>
-      <c r="R25" s="24" t="inlineStr">
+      <c r="R25" s="22" t="inlineStr">
         <is>
           <t>Lukas</t>
         </is>
       </c>
-      <c r="S25" s="24" t="inlineStr">
+      <c r="S25" s="22" t="inlineStr">
         <is>
           <t>Dana</t>
         </is>
       </c>
-      <c r="T25" s="27" t="inlineStr">
+      <c r="T25" s="23" t="inlineStr">
         <is>
           <t>Alex</t>
         </is>
       </c>
-      <c r="U25" s="27" t="inlineStr">
+      <c r="U25" s="23" t="inlineStr">
         <is>
           <t>Gabriela</t>
         </is>
@@ -3586,12 +3608,12 @@
         </is>
       </c>
       <c r="G26" s="11" t="n"/>
-      <c r="H26" s="25" t="inlineStr">
+      <c r="H26" s="23" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I26" s="25" t="inlineStr">
+      <c r="I26" s="23" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
@@ -3602,12 +3624,12 @@
         </is>
       </c>
       <c r="K26" s="11" t="n"/>
-      <c r="L26" s="25" t="inlineStr">
+      <c r="L26" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M26" s="25" t="inlineStr">
+      <c r="M26" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
@@ -3661,12 +3683,12 @@
         </is>
       </c>
       <c r="G27" s="11" t="n"/>
-      <c r="H27" s="25" t="inlineStr">
+      <c r="H27" s="23" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I27" s="25" t="inlineStr">
+      <c r="I27" s="23" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
@@ -3677,12 +3699,12 @@
         </is>
       </c>
       <c r="K27" s="11" t="n"/>
-      <c r="L27" s="25" t="inlineStr">
+      <c r="L27" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M27" s="25" t="inlineStr">
+      <c r="M27" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>
@@ -3736,12 +3758,12 @@
         </is>
       </c>
       <c r="G28" s="11" t="n"/>
-      <c r="H28" s="25" t="inlineStr">
+      <c r="H28" s="23" t="inlineStr">
         <is>
           <t>Ozan</t>
         </is>
       </c>
-      <c r="I28" s="25" t="inlineStr">
+      <c r="I28" s="23" t="inlineStr">
         <is>
           <t>Anastasia</t>
         </is>
@@ -3752,12 +3774,12 @@
         </is>
       </c>
       <c r="K28" s="11" t="n"/>
-      <c r="L28" s="25" t="inlineStr">
+      <c r="L28" s="23" t="inlineStr">
         <is>
           <t>Chris</t>
         </is>
       </c>
-      <c r="M28" s="25" t="inlineStr">
+      <c r="M28" s="23" t="inlineStr">
         <is>
           <t>Emmy</t>
         </is>

</xml_diff>